<commit_message>
changed label mode in loading to binary
</commit_message>
<xml_diff>
--- a/дипломна работа стойности.xlsx
+++ b/дипломна работа стойности.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="72" windowWidth="14340" windowHeight="8496"/>
+    <workbookView xWindow="288" yWindow="72" windowWidth="11232" windowHeight="5220"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Epoch</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Testing Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training Loss </t>
+  </si>
+  <si>
+    <t>Validation Loss</t>
   </si>
 </sst>
 </file>
@@ -87,10 +93,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="110"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="10"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -105,20 +111,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Xception</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> network results</a:t>
+              <a:t>Xception network results</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -625,11 +624,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174810624"/>
-        <c:axId val="173265408"/>
+        <c:axId val="171175936"/>
+        <c:axId val="163139520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174810624"/>
+        <c:axId val="171175936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +657,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173265408"/>
+        <c:crossAx val="163139520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -666,9 +665,667 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173265408"/>
+        <c:axId val="163139520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy, %</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="171175936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="bg-BG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Modified</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Xception results</a:t>
+            </a:r>
+            <a:endParaRPr lang="bg-BG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$49:$B$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>79.709999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94.72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>95.18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>94.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>95.23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>96.17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95.83</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95.85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>96.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>96.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>97.32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>96.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>96.68</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>96.86</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>96.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>97.28</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>97.61</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97.52</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>97.14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>97.66</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>97.57</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>98.22</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>98.08</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>98.36</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>99.11</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>97.99</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>97.8</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>98.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>98.36</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>97.8</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>98.22</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>98.55</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>98.46</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>98.64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>99.06</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>98.64</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>98.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>98.64</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>99.3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>98.97</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>99.2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>99.44</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>98.78</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>98.83</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>99.11</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>99.2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>99.63</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>99.11</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>99.63</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>99.63</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>99.49</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>98.92</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>99.58</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>99.34</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>99.39</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>99.3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>99.2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>99.02</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>99.63</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>99.58</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>99.49</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>99.44</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>99.16</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>99.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$49:$C$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>50.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.73</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92.87</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84.43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>92.87</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>90.24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.87</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94.18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>94.93</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>94.56</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>94.75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>94.56</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>94.18</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>81.99</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>96.06</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>65.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>95.87</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>94.93</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>96.62</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>78.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>96.25</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>93.62</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>94.37</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>95.68</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>93.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95.68</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>96.44</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>95.12</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>88.56</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>96.06</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95.68</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>95.68</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>91.56</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>94.93</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>96.62</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>89.87</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>95.12</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>96.62</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>95.12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>96.06</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>95.87</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>91.37</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>96.81</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>96.25</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>95.12</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>93.81</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>96.44</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>88.93</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>96.44</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>95.68</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>79.55</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>96.06</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>94.56</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>95.87</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>97.19</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>85.74</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>95.68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>92.5</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>88.93</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>93.62</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>94.75</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>92.68</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>94.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="171177472"/>
+        <c:axId val="163142976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="171177472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Epoch</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:crossAx val="163142976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="163142976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -701,9 +1358,644 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174810624"/>
+        <c:crossAx val="171177472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="bg-BG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Modified</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Xception loss function</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training Loss </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$49:$D$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.43580000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2747</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26229999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2167</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2077</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.17879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1535</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15939999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1341</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13120000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1036</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1114</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.1105</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.8599999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.6199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.6100000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.2799999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.7199999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.5800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.3799999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.9699999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.5500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.8600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.5500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.21E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.8099999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.7300000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.8600000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.7000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.0799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.41E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.0899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.5500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.21E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.7600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.7100000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.9899999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.85E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.9399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.2700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.0300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.6799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.61E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.93E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.3699999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.9499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.7500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.49E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.84E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.12E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.3199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.58E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.1000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.4800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.44E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.7399999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Validation Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$E$49:$E$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.79769999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2128999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54720000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0801000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3886</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6349</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.19309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43980000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1691</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1767</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.18859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2467</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25890000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16719999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16259999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2014</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1363</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.22409999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.15079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.54069999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.93689999999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.15590000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.12870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.11840000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.78900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.2306</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.21940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.21110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.3899999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.219</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.19040000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.0700000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.13619999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.30130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.1108</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.1056</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.19620000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.16769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.1096</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.27629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.16589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.4299999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.14360000000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.34320000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.1173</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.1285</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.22109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.26850000000000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>8.1600000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.4133</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.1104</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.11360000000000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.12570000000000001</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.53959999999999997</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.1547</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.18440000000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.10879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.6400000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.54279999999999995</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.15670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.26779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.40849999999999997</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.29659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.21759999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.26029999999999998</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.26729999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="171177984"/>
+        <c:axId val="214468864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="171177984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="214468864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="214468864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Loss  function</a:t>
+                </a:r>
+                <a:endParaRPr lang="bg-BG"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="171177984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -728,15 +2020,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>430306</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>143436</xdr:rowOff>
+      <xdr:colOff>905436</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>44825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>403411</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -750,6 +2042,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>286871</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>14668</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>600634</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>140990</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193963</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>170328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>600635</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>71717</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграма 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1045,17 +2397,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE55" sqref="AE55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1506,7 +2859,7 @@
         <v>70.83</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1520,7 +2873,7 @@
         <v>75.48</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1534,7 +2887,7 @@
         <v>81.09</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1548,7 +2901,7 @@
         <v>77.88</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1562,7 +2915,7 @@
         <v>78.849999999999994</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1576,7 +2929,7 @@
         <v>78.37</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1590,7 +2943,7 @@
         <v>76.44</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1604,7 +2957,7 @@
         <v>78.040000000000006</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1618,7 +2971,7 @@
         <v>70.19</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1632,7 +2985,7 @@
         <v>71.959999999999994</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1646,7 +2999,7 @@
         <v>78.37</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1660,7 +3013,7 @@
         <v>68.91</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1674,7 +3027,7 @@
         <v>79.010000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1688,7 +3041,7 @@
         <v>74.84</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1700,6 +3053,1300 @@
       </c>
       <c r="D46">
         <v>82.53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>79.709999999999994</v>
+      </c>
+      <c r="C49">
+        <v>50.84</v>
+      </c>
+      <c r="D49">
+        <v>0.43580000000000002</v>
+      </c>
+      <c r="E49">
+        <v>0.79769999999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>89.32</v>
+      </c>
+      <c r="C50">
+        <v>50.84</v>
+      </c>
+      <c r="D50">
+        <v>0.2747</v>
+      </c>
+      <c r="E50">
+        <v>2.2128999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>90.02</v>
+      </c>
+      <c r="C51">
+        <v>67.73</v>
+      </c>
+      <c r="D51">
+        <v>0.26229999999999998</v>
+      </c>
+      <c r="E51">
+        <v>0.54720000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>91.56</v>
+      </c>
+      <c r="C52">
+        <v>58.91</v>
+      </c>
+      <c r="D52">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="E52">
+        <v>1.0801000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>91.71</v>
+      </c>
+      <c r="C53">
+        <v>83.3</v>
+      </c>
+      <c r="D53">
+        <v>0.2167</v>
+      </c>
+      <c r="E53">
+        <v>0.3886</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>92.79</v>
+      </c>
+      <c r="C54">
+        <v>53.85</v>
+      </c>
+      <c r="D54">
+        <v>0.2077</v>
+      </c>
+      <c r="E54">
+        <v>1.6349</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <v>93.77</v>
+      </c>
+      <c r="C55">
+        <v>92.87</v>
+      </c>
+      <c r="D55">
+        <v>0.17879999999999999</v>
+      </c>
+      <c r="E55">
+        <v>0.19309999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>8</v>
+      </c>
+      <c r="B56">
+        <v>94.91</v>
+      </c>
+      <c r="C56">
+        <v>84.43</v>
+      </c>
+      <c r="D56">
+        <v>0.1535</v>
+      </c>
+      <c r="E56">
+        <v>0.43980000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>94.45</v>
+      </c>
+      <c r="C57">
+        <v>94</v>
+      </c>
+      <c r="D57">
+        <v>0.15939999999999999</v>
+      </c>
+      <c r="E57">
+        <v>0.1691</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>95.5</v>
+      </c>
+      <c r="C58">
+        <v>94.56</v>
+      </c>
+      <c r="D58">
+        <v>0.1341</v>
+      </c>
+      <c r="E58">
+        <v>0.1767</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>11</v>
+      </c>
+      <c r="B59">
+        <v>94.72</v>
+      </c>
+      <c r="C59">
+        <v>92.87</v>
+      </c>
+      <c r="D59">
+        <v>0.15670000000000001</v>
+      </c>
+      <c r="E59">
+        <v>0.18859999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>12</v>
+      </c>
+      <c r="B60">
+        <v>95.18</v>
+      </c>
+      <c r="C60">
+        <v>90.24</v>
+      </c>
+      <c r="D60">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E60">
+        <v>0.2467</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>13</v>
+      </c>
+      <c r="B61">
+        <v>94.92</v>
+      </c>
+      <c r="C61">
+        <v>89.87</v>
+      </c>
+      <c r="D61">
+        <v>0.13120000000000001</v>
+      </c>
+      <c r="E61">
+        <v>0.25890000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>14</v>
+      </c>
+      <c r="B62">
+        <v>95.23</v>
+      </c>
+      <c r="C62">
+        <v>94.18</v>
+      </c>
+      <c r="D62">
+        <v>0.14069999999999999</v>
+      </c>
+      <c r="E62">
+        <v>0.16719999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>15</v>
+      </c>
+      <c r="B63">
+        <v>96.17</v>
+      </c>
+      <c r="C63">
+        <v>94.18</v>
+      </c>
+      <c r="D63">
+        <f>1036/10000</f>
+        <v>0.1036</v>
+      </c>
+      <c r="E63">
+        <v>0.16259999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>16</v>
+      </c>
+      <c r="B64">
+        <v>95.83</v>
+      </c>
+      <c r="C64">
+        <v>94.93</v>
+      </c>
+      <c r="D64">
+        <f>1114/10000</f>
+        <v>0.1114</v>
+      </c>
+      <c r="E64">
+        <v>0.2014</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>17</v>
+      </c>
+      <c r="B65">
+        <v>95.85</v>
+      </c>
+      <c r="C65">
+        <v>94.56</v>
+      </c>
+      <c r="D65">
+        <v>0.1105</v>
+      </c>
+      <c r="E65">
+        <v>0.15659999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>18</v>
+      </c>
+      <c r="B66">
+        <v>96.9</v>
+      </c>
+      <c r="C66">
+        <v>94.75</v>
+      </c>
+      <c r="D66">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="E66">
+        <v>0.1363</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>19</v>
+      </c>
+      <c r="B67">
+        <v>96.6</v>
+      </c>
+      <c r="C67">
+        <v>90.06</v>
+      </c>
+      <c r="D67">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E67">
+        <v>0.22409999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>20</v>
+      </c>
+      <c r="B68">
+        <v>97.32</v>
+      </c>
+      <c r="C68">
+        <v>94.56</v>
+      </c>
+      <c r="D68">
+        <v>9.6199999999999994E-2</v>
+      </c>
+      <c r="E68">
+        <v>0.15079999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>21</v>
+      </c>
+      <c r="B69">
+        <v>96.4</v>
+      </c>
+      <c r="C69">
+        <v>94.18</v>
+      </c>
+      <c r="D69">
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="E69">
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>22</v>
+      </c>
+      <c r="B70">
+        <v>96.68</v>
+      </c>
+      <c r="C70">
+        <v>81.99</v>
+      </c>
+      <c r="D70">
+        <v>9.2799999999999994E-2</v>
+      </c>
+      <c r="E70">
+        <v>0.54069999999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>23</v>
+      </c>
+      <c r="B71">
+        <v>96.86</v>
+      </c>
+      <c r="C71">
+        <v>96.06</v>
+      </c>
+      <c r="D71">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E71">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>24</v>
+      </c>
+      <c r="B72">
+        <v>96.4</v>
+      </c>
+      <c r="C72">
+        <v>65.290000000000006</v>
+      </c>
+      <c r="D72">
+        <v>9.7199999999999995E-2</v>
+      </c>
+      <c r="E72">
+        <v>0.93689999999999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>25</v>
+      </c>
+      <c r="B73">
+        <v>97.28</v>
+      </c>
+      <c r="C73">
+        <v>95.87</v>
+      </c>
+      <c r="D73">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="E73">
+        <v>0.15590000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>26</v>
+      </c>
+      <c r="B74">
+        <v>98.03</v>
+      </c>
+      <c r="C74">
+        <v>94.93</v>
+      </c>
+      <c r="D74">
+        <v>6.3799999999999996E-2</v>
+      </c>
+      <c r="E74">
+        <v>0.12870000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>27</v>
+      </c>
+      <c r="B75">
+        <v>97.61</v>
+      </c>
+      <c r="C75">
+        <v>96.62</v>
+      </c>
+      <c r="D75">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="E75">
+        <v>0.11840000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>28</v>
+      </c>
+      <c r="B76">
+        <v>97.52</v>
+      </c>
+      <c r="C76">
+        <v>78.8</v>
+      </c>
+      <c r="D76">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="E76">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>29</v>
+      </c>
+      <c r="B77">
+        <v>97.14</v>
+      </c>
+      <c r="C77">
+        <v>96.25</v>
+      </c>
+      <c r="D77">
+        <v>7.8600000000000003E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>30</v>
+      </c>
+      <c r="B78">
+        <v>97.66</v>
+      </c>
+      <c r="C78">
+        <v>93.62</v>
+      </c>
+      <c r="D78">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E78">
+        <v>0.2306</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>31</v>
+      </c>
+      <c r="B79">
+        <v>97.57</v>
+      </c>
+      <c r="C79">
+        <v>94</v>
+      </c>
+      <c r="D79">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="E79">
+        <v>0.21940000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>32</v>
+      </c>
+      <c r="B80">
+        <v>98.22</v>
+      </c>
+      <c r="C80">
+        <v>94.37</v>
+      </c>
+      <c r="D80">
+        <v>0.06</v>
+      </c>
+      <c r="E80">
+        <v>0.21110000000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>33</v>
+      </c>
+      <c r="B81">
+        <v>98.03</v>
+      </c>
+      <c r="C81">
+        <v>95.68</v>
+      </c>
+      <c r="D81">
+        <v>5.21E-2</v>
+      </c>
+      <c r="E81">
+        <v>9.3899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>34</v>
+      </c>
+      <c r="B82">
+        <v>98.08</v>
+      </c>
+      <c r="C82">
+        <v>93.25</v>
+      </c>
+      <c r="D82">
+        <v>5.8099999999999999E-2</v>
+      </c>
+      <c r="E82">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>35</v>
+      </c>
+      <c r="B83">
+        <v>98.36</v>
+      </c>
+      <c r="C83">
+        <v>95.68</v>
+      </c>
+      <c r="D83">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="E83">
+        <v>0.19040000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>36</v>
+      </c>
+      <c r="B84">
+        <v>99.11</v>
+      </c>
+      <c r="C84">
+        <v>96.44</v>
+      </c>
+      <c r="D84">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="E84">
+        <v>9.0700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>37</v>
+      </c>
+      <c r="B85">
+        <v>97.99</v>
+      </c>
+      <c r="C85">
+        <v>95.12</v>
+      </c>
+      <c r="D85">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E85">
+        <v>0.13619999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>38</v>
+      </c>
+      <c r="B86">
+        <v>97.8</v>
+      </c>
+      <c r="C86">
+        <v>88.56</v>
+      </c>
+      <c r="D86">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="E86">
+        <v>0.30130000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>39</v>
+      </c>
+      <c r="B87">
+        <v>98.6</v>
+      </c>
+      <c r="C87">
+        <v>96.06</v>
+      </c>
+      <c r="D87">
+        <v>4.41E-2</v>
+      </c>
+      <c r="E87">
+        <v>0.1108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>40</v>
+      </c>
+      <c r="B88">
+        <v>98.36</v>
+      </c>
+      <c r="C88">
+        <v>95.68</v>
+      </c>
+      <c r="D88">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="E88">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>41</v>
+      </c>
+      <c r="B89">
+        <v>97.8</v>
+      </c>
+      <c r="C89">
+        <v>95.68</v>
+      </c>
+      <c r="D89">
+        <v>5.5500000000000001E-2</v>
+      </c>
+      <c r="E89">
+        <v>0.1056</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>42</v>
+      </c>
+      <c r="B90">
+        <v>98.22</v>
+      </c>
+      <c r="C90">
+        <v>91.56</v>
+      </c>
+      <c r="D90">
+        <v>5.21E-2</v>
+      </c>
+      <c r="E90">
+        <v>0.19620000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>43</v>
+      </c>
+      <c r="B91">
+        <v>98.55</v>
+      </c>
+      <c r="C91">
+        <v>94.93</v>
+      </c>
+      <c r="D91">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="E91">
+        <v>0.16769999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>44</v>
+      </c>
+      <c r="B92">
+        <v>98.46</v>
+      </c>
+      <c r="C92">
+        <v>96.62</v>
+      </c>
+      <c r="D92">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="E92">
+        <v>0.1096</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>45</v>
+      </c>
+      <c r="B93">
+        <v>98.64</v>
+      </c>
+      <c r="C93">
+        <v>89.87</v>
+      </c>
+      <c r="D93">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="E93">
+        <v>0.27629999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>46</v>
+      </c>
+      <c r="B94">
+        <v>99.06</v>
+      </c>
+      <c r="C94">
+        <v>95.12</v>
+      </c>
+      <c r="D94">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E94">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>47</v>
+      </c>
+      <c r="B95">
+        <v>98.64</v>
+      </c>
+      <c r="C95">
+        <v>96.62</v>
+      </c>
+      <c r="D95">
+        <v>3.85E-2</v>
+      </c>
+      <c r="E95">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>48</v>
+      </c>
+      <c r="B96">
+        <v>98.6</v>
+      </c>
+      <c r="C96">
+        <v>95.12</v>
+      </c>
+      <c r="D96">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="E96">
+        <v>0.16589999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>49</v>
+      </c>
+      <c r="B97">
+        <v>98.64</v>
+      </c>
+      <c r="C97">
+        <v>96.06</v>
+      </c>
+      <c r="D97">
+        <v>4.2700000000000002E-2</v>
+      </c>
+      <c r="E97">
+        <v>9.4299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>50</v>
+      </c>
+      <c r="B98">
+        <v>99.3</v>
+      </c>
+      <c r="C98">
+        <v>95.87</v>
+      </c>
+      <c r="D98">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E98">
+        <v>0.14360000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>51</v>
+      </c>
+      <c r="B99">
+        <v>98.97</v>
+      </c>
+      <c r="C99">
+        <v>91.37</v>
+      </c>
+      <c r="D99">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E99">
+        <v>0.34320000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>52</v>
+      </c>
+      <c r="B100">
+        <v>99.2</v>
+      </c>
+      <c r="C100">
+        <v>96.81</v>
+      </c>
+      <c r="D100">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E100">
+        <v>0.1173</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>53</v>
+      </c>
+      <c r="B101">
+        <v>99.44</v>
+      </c>
+      <c r="C101">
+        <v>96.25</v>
+      </c>
+      <c r="D101">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="E101">
+        <v>0.1285</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>54</v>
+      </c>
+      <c r="B102">
+        <v>98.78</v>
+      </c>
+      <c r="C102">
+        <v>95.12</v>
+      </c>
+      <c r="D102">
+        <v>3.61E-2</v>
+      </c>
+      <c r="E102">
+        <v>0.22109999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>55</v>
+      </c>
+      <c r="B103">
+        <v>98.83</v>
+      </c>
+      <c r="C103">
+        <v>92.5</v>
+      </c>
+      <c r="D103">
+        <v>2.93E-2</v>
+      </c>
+      <c r="E103">
+        <v>0.26850000000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>56</v>
+      </c>
+      <c r="B104">
+        <v>99.11</v>
+      </c>
+      <c r="C104">
+        <v>93.81</v>
+      </c>
+      <c r="D104">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="E104">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>57</v>
+      </c>
+      <c r="B105">
+        <v>99.2</v>
+      </c>
+      <c r="C105">
+        <v>96.44</v>
+      </c>
+      <c r="D105">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="E105">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>58</v>
+      </c>
+      <c r="B106">
+        <v>99.63</v>
+      </c>
+      <c r="C106">
+        <v>88.93</v>
+      </c>
+      <c r="D106">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E106">
+        <v>0.4133</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>59</v>
+      </c>
+      <c r="B107">
+        <v>99.11</v>
+      </c>
+      <c r="C107">
+        <v>96.44</v>
+      </c>
+      <c r="D107">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="E107">
+        <v>0.1104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>60</v>
+      </c>
+      <c r="B108">
+        <v>99.63</v>
+      </c>
+      <c r="C108">
+        <v>97</v>
+      </c>
+      <c r="D108">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="E108">
+        <v>0.11360000000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>61</v>
+      </c>
+      <c r="B109">
+        <v>99.63</v>
+      </c>
+      <c r="C109">
+        <v>97</v>
+      </c>
+      <c r="D109">
+        <v>1.49E-2</v>
+      </c>
+      <c r="E109">
+        <v>0.12570000000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>62</v>
+      </c>
+      <c r="B110">
+        <v>99.49</v>
+      </c>
+      <c r="C110">
+        <v>95.68</v>
+      </c>
+      <c r="D110">
+        <v>1.84E-2</v>
+      </c>
+      <c r="E110">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>63</v>
+      </c>
+      <c r="B111">
+        <v>98.92</v>
+      </c>
+      <c r="C111">
+        <v>79.55</v>
+      </c>
+      <c r="D111">
+        <v>3.09E-2</v>
+      </c>
+      <c r="E111">
+        <v>0.53959999999999997</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>64</v>
+      </c>
+      <c r="B112">
+        <v>99.58</v>
+      </c>
+      <c r="C112">
+        <v>96.06</v>
+      </c>
+      <c r="D112">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="E112">
+        <v>0.1547</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>65</v>
+      </c>
+      <c r="B113">
+        <v>99.34</v>
+      </c>
+      <c r="C113">
+        <v>94.56</v>
+      </c>
+      <c r="D113">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="E113">
+        <v>0.18440000000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>66</v>
+      </c>
+      <c r="B114">
+        <v>99.39</v>
+      </c>
+      <c r="C114">
+        <v>95.87</v>
+      </c>
+      <c r="D114">
+        <v>2.12E-2</v>
+      </c>
+      <c r="E114">
+        <v>0.10879999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>67</v>
+      </c>
+      <c r="B115">
+        <v>99.3</v>
+      </c>
+      <c r="C115">
+        <v>97.19</v>
+      </c>
+      <c r="D115">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="E115">
+        <v>8.6400000000000005E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>68</v>
+      </c>
+      <c r="B116">
+        <v>99.2</v>
+      </c>
+      <c r="C116">
+        <v>85.74</v>
+      </c>
+      <c r="D116">
+        <v>2.58E-2</v>
+      </c>
+      <c r="E116">
+        <v>0.54279999999999995</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>69</v>
+      </c>
+      <c r="B117">
+        <v>99.02</v>
+      </c>
+      <c r="C117">
+        <v>95.68</v>
+      </c>
+      <c r="D117">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E117">
+        <v>0.15670000000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>70</v>
+      </c>
+      <c r="B118">
+        <v>99.63</v>
+      </c>
+      <c r="C118">
+        <v>92.5</v>
+      </c>
+      <c r="D118">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E118">
+        <v>0.26779999999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>71</v>
+      </c>
+      <c r="B119">
+        <v>99.58</v>
+      </c>
+      <c r="C119">
+        <v>88.93</v>
+      </c>
+      <c r="D119">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="E119">
+        <v>0.40849999999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>72</v>
+      </c>
+      <c r="B120">
+        <v>99.49</v>
+      </c>
+      <c r="C120">
+        <v>93.62</v>
+      </c>
+      <c r="D120">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E120">
+        <v>0.29659999999999997</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>73</v>
+      </c>
+      <c r="B121">
+        <v>99.44</v>
+      </c>
+      <c r="C121">
+        <v>94.75</v>
+      </c>
+      <c r="D121">
+        <v>1.44E-2</v>
+      </c>
+      <c r="E121">
+        <v>0.21759999999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>74</v>
+      </c>
+      <c r="B122">
+        <v>99.16</v>
+      </c>
+      <c r="C122">
+        <v>92.68</v>
+      </c>
+      <c r="D122">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E122">
+        <v>0.26029999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>75</v>
+      </c>
+      <c r="B123">
+        <v>99.53</v>
+      </c>
+      <c r="C123">
+        <v>94.56</v>
+      </c>
+      <c r="D123">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="E123">
+        <v>0.26729999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>